<commit_message>
Update QA Challenge - Chicks Gold.xlsx
</commit_message>
<xml_diff>
--- a/test-cases/QA Challenge - Chicks Gold.xlsx
+++ b/test-cases/QA Challenge - Chicks Gold.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27927"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C64D5AA2-AB87-4269-8326-ABA61432C35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D863F589-30FD-48CA-A4C2-80464E0462F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Authentication" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="546">
   <si>
     <t>Project Name:</t>
   </si>
@@ -237,8 +237,7 @@
 2. The user has already logged in</t>
   </si>
   <si>
-    <t>Find a "Logout" button
-Be logged out when click it</t>
+    <t>Find a "Logout" button. Be logged out when click it</t>
   </si>
   <si>
     <t>1. There is no "Logout" button
@@ -333,6 +332,9 @@
     <t>Product Management</t>
   </si>
   <si>
+    <t>TC_010</t>
+  </si>
+  <si>
     <t>Create a new product with all required fields</t>
   </si>
   <si>
@@ -353,9 +355,12 @@
     <t>Product is successfully created and appears in the Product List</t>
   </si>
   <si>
-    <t>1. In the products page it only displays &lt;h2&gt;Product List&lt;/h2&gt;
+    <t>1. In the products page it is only displayed &lt;h2&gt;Product List&lt;/h2&gt;
 2. There is not a "Create Product" button
 3. The Product List is empty and user can not add any product</t>
+  </si>
+  <si>
+    <t>TC_011</t>
   </si>
   <si>
     <t xml:space="preserve"> Update information for an existing product</t>
@@ -380,10 +385,13 @@
     <t>Product information is successfully updated and changes are reflected in the Product List</t>
   </si>
   <si>
-    <t>1. In the products page it only displays &lt;h2&gt;Product List&lt;/h2&gt;
+    <t>1. In the products page it is only displayed &lt;h2&gt;Product List&lt;/h2&gt;
 2. User cannot see an "Edit" button
-·User cannot see a "Save Changes" button
-3. The Product List is empty and user can not add any product</t>
+3. User cannot see a "Save Changes" button
+4. The Product List is empty and user can not add any product</t>
+  </si>
+  <si>
+    <t>TC_012</t>
   </si>
   <si>
     <t xml:space="preserve"> Delete a product</t>
@@ -409,6 +417,9 @@
 2. User cannot see an "Delete" button</t>
   </si>
   <si>
+    <t>TC_013</t>
+  </si>
+  <si>
     <t>Get list of all products</t>
   </si>
   <si>
@@ -426,6 +437,9 @@
   </si>
   <si>
     <t>1. User cannot see product displayed</t>
+  </si>
+  <si>
+    <t>TC_0014</t>
   </si>
   <si>
     <t xml:space="preserve"> Search products by category</t>
@@ -449,7 +463,10 @@
   </si>
   <si>
     <t>1. User cannot see a category filter
-2.User cannot see products displayed</t>
+2. User cannot see products displayed</t>
+  </si>
+  <si>
+    <t>TC_015</t>
   </si>
   <si>
     <t xml:space="preserve"> Search products by name or description</t>
@@ -477,6 +494,9 @@
 2. User cannot see products displayed</t>
   </si>
   <si>
+    <t>TC_016</t>
+  </si>
+  <si>
     <t>Verify access to protected routes without authentication token</t>
   </si>
   <si>
@@ -501,6 +521,9 @@
 3. No error message appears</t>
   </si>
   <si>
+    <t>TC_017</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Verify that only authorized users can modify products</t>
   </si>
   <si>
@@ -530,6 +553,9 @@
   </si>
   <si>
     <t>Order Processing</t>
+  </si>
+  <si>
+    <t>TC_018</t>
   </si>
   <si>
     <t>Create a new order with valid products</t>
@@ -557,11 +583,14 @@
     <t>Order is successfully created and appears in the user's order history</t>
   </si>
   <si>
-    <t>1. In the orders page it only displays &lt;h2&gt;Order List&lt;/h2&gt;
+    <t>1. In the orders page it  s only displayed &lt;h2&gt;Order List&lt;/h2&gt;
 2. User cannot see a shopping cart
 3. User cannot see a checkout section
 4. User cannot see a form to fill in order details
 5. User cannot see a button to confirm the order</t>
+  </si>
+  <si>
+    <t>TC_019</t>
   </si>
   <si>
     <t>Update the status of an order</t>
@@ -592,6 +621,9 @@
 4. User cannot see a "Save changes" button</t>
   </si>
   <si>
+    <t>TC_020</t>
+  </si>
+  <si>
     <t>Cancel an order</t>
   </si>
   <si>
@@ -621,6 +653,9 @@
 5. User cannot see a button to confirm the cancellation</t>
   </si>
   <si>
+    <t>TC_021</t>
+  </si>
+  <si>
     <t>Get list of orders from a user</t>
   </si>
   <si>
@@ -643,6 +678,9 @@
   <si>
     <t>1. There is no an order history
 2. User cannot see a list of existing orders</t>
+  </si>
+  <si>
+    <t>TC_022</t>
   </si>
   <si>
     <t>Get details of a specific order</t>
@@ -671,6 +709,9 @@
 3. User cannot see order details</t>
   </si>
   <si>
+    <t>TC_023</t>
+  </si>
+  <si>
     <t>Verify correct calculation of the order total</t>
   </si>
   <si>
@@ -697,6 +738,9 @@
 3. User cannot see products prices</t>
   </si>
   <si>
+    <t>TC_024</t>
+  </si>
+  <si>
     <t>Process payment for an order (simulated)</t>
   </si>
   <si>
@@ -719,7 +763,7 @@
   </si>
   <si>
     <t>1. User cannot create a new order
-2. PUser cannot see a payment section
+2. User cannot see a payment section
 3. User cannot see a form to fill payment details
 4. User cannot see a button to confirm a payment</t>
   </si>
@@ -728,6 +772,9 @@
   </si>
   <si>
     <t>User Authentication and Dashboard</t>
+  </si>
+  <si>
+    <t>TC_025</t>
   </si>
   <si>
     <t>Login with valid credentials</t>
@@ -753,6 +800,9 @@
     <t>User is successful logged in but not redirected to the dashboard</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
     <t>Show success message for successful login</t>
   </si>
   <si>
@@ -767,6 +817,9 @@
   </si>
   <si>
     <t>Message "Logged in with token: sampletoken" is shown after login</t>
+  </si>
+  <si>
+    <t>TC_027</t>
   </si>
   <si>
     <t>Show error message for invalid credentials</t>
@@ -790,6 +843,9 @@
     <t>Message "Login failed" is shown after attemp to log in with invalid credebtials</t>
   </si>
   <si>
+    <t>TC_028</t>
+  </si>
+  <si>
     <t>Log out from the dashboard</t>
   </si>
   <si>
@@ -815,6 +871,9 @@
 2. User cannot log out  from the system</t>
   </si>
   <si>
+    <t>TC_029</t>
+  </si>
+  <si>
     <t>View user profile information</t>
   </si>
   <si>
@@ -834,6 +893,9 @@
   <si>
     <t>1. User cannot see a profile section
 3. User cannot see displayed information</t>
+  </si>
+  <si>
+    <t>TC_030</t>
   </si>
   <si>
     <t>Edit user profile information</t>
@@ -861,6 +923,9 @@
 5. User cannot see a "Save the changes" button</t>
   </si>
   <si>
+    <t>TC_031</t>
+  </si>
+  <si>
     <t xml:space="preserve">Verify that the dashboard displays relevant information </t>
   </si>
   <si>
@@ -881,6 +946,9 @@
   <si>
     <t>1. Dashboard only displays the message "Welcome to the user dashboard!"
 2. Dashboard do not display any relevant information</t>
+  </si>
+  <si>
+    <t>TC_032</t>
   </si>
   <si>
     <t>Verify user dashboard data display</t>
@@ -908,6 +976,9 @@
 2. Dashboard do not display any section nor information of the user activities</t>
   </si>
   <si>
+    <t>TC_033</t>
+  </si>
+  <si>
     <t>Verify user dashboard data refresh</t>
   </si>
   <si>
@@ -941,6 +1012,9 @@
     <t>Product Listing-Order Processing</t>
   </si>
   <si>
+    <t>TC_034</t>
+  </si>
+  <si>
     <t>Load and display product list correctly</t>
   </si>
   <si>
@@ -966,6 +1040,9 @@
 3. User cannot see pagination </t>
   </si>
   <si>
+    <t>TC_035</t>
+  </si>
+  <si>
     <t>Filter products by category</t>
   </si>
   <si>
@@ -990,6 +1067,9 @@
     <t>1. In the products page it only displays &lt;h2&gt;Product List&lt;/h2&gt;
 2. User cannot see products displayed
 3. User cannot see categories</t>
+  </si>
+  <si>
+    <t>TC_036</t>
   </si>
   <si>
     <t>Search products by name</t>
@@ -1019,6 +1099,9 @@
 2. User cannot see a search field</t>
   </si>
   <si>
+    <t>TC_037</t>
+  </si>
+  <si>
     <t>Add products to shopping cart</t>
   </si>
   <si>
@@ -1046,6 +1129,9 @@
 2. User cannot see an "Add to Cart" button
 3. User cannot see a shopping cart
 4. User cannot add products to the cart</t>
+  </si>
+  <si>
+    <t>TC_038</t>
   </si>
   <si>
     <t>Modify quantity of products in the cart</t>
@@ -1078,6 +1164,9 @@
 5. User cannot modify the quantity of products</t>
   </si>
   <si>
+    <t>TC_039</t>
+  </si>
+  <si>
     <t>Remove products from cart</t>
   </si>
   <si>
@@ -1098,10 +1187,12 @@
 3. Visual confirmation is displayed that the product has been removed</t>
   </si>
   <si>
-    <t xml:space="preserve">1. User cannot see a list of products
+    <t>1. User cannot see a list of products
 2. User cannot see a "Delete" or "Remove from Cart" button
-3. User cannot delete a product from the cart
-</t>
+3. User cannot delete a product from the cart</t>
+  </si>
+  <si>
+    <t>TC_040</t>
   </si>
   <si>
     <t>Process an order from the cart</t>
@@ -1131,11 +1222,13 @@
 4. The cart is emptied after the order is processed</t>
   </si>
   <si>
-    <t xml:space="preserve">1. User cannot add products to cart
+    <t>1. User cannot add products to cart
 2. User cannot see a checkout page
 3. User cannot see a form to fill in the necessary information (shipping address, payment method, etc.)
-4. User cannot confirm the order
-</t>
+4. User cannot confirm the order</t>
+  </si>
+  <si>
+    <t>TC_041</t>
   </si>
   <si>
     <t>View order history</t>
@@ -1160,9 +1253,11 @@
 3. Orders are displayed in reverse chronological order (most recent first)</t>
   </si>
   <si>
-    <t xml:space="preserve">1. User cannot see an "Order History" section
-2. User cannot see a list of previous orders
-</t>
+    <t>1. User cannot see an "Order History" section
+2. User cannot see a list of previous orders</t>
+  </si>
+  <si>
+    <t>TC_042</t>
   </si>
   <si>
     <t>View details of a specific order</t>
@@ -1200,6 +1295,9 @@
     <t>Integration Testing</t>
   </si>
   <si>
+    <t>TC_043</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Verify that the products created in the backend appear in the Aurelia list</t>
   </si>
   <si>
@@ -1226,6 +1324,9 @@
 2. User do not have access to create products</t>
   </si>
   <si>
+    <t>TC_044</t>
+  </si>
+  <si>
     <t>Check that orders placed in Aurelia are reflected in the ReactJS dashboard</t>
   </si>
   <si>
@@ -1250,6 +1351,9 @@
     <t>1. User cannot shop products, they cannot see products nor buttons to interact with</t>
   </si>
   <si>
+    <t>TC_045</t>
+  </si>
+  <si>
     <t>Ensure that order status changes on the backend will be updated in real time on the frontend</t>
   </si>
   <si>
@@ -1272,13 +1376,16 @@
 2. The state change is also updated in real time in the ReactJS dashboard</t>
   </si>
   <si>
-    <t>User cannot make orders, nor buy products</t>
+    <t>User cannot place orders, nor buy products</t>
   </si>
   <si>
     <t>Perf_001</t>
   </si>
   <si>
     <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>TC_046</t>
   </si>
   <si>
     <t>Measure response time to load the product list with 100, 1000 and 10000 products</t>
@@ -1305,6 +1412,9 @@
   </si>
   <si>
     <t>As a tester, I cannot load products on the page because there are no buttons nor interactivity in the Products and Orders pages</t>
+  </si>
+  <si>
+    <t>TC_047</t>
   </si>
   <si>
     <t>Evaluate order processing time under load (50 simultaneous orders)</t>
@@ -1332,6 +1442,9 @@
 3. System resources (CPU, memory, database) remain stable during the test</t>
   </si>
   <si>
+    <t>TC_048</t>
+  </si>
+  <si>
     <t>Measure login time with 100 concurrent users</t>
   </si>
   <si>
@@ -1358,13 +1471,16 @@
 4. me daAny outliers in login times are identified for further investigation</t>
   </si>
   <si>
-    <t>As a Tester I cannot execute this test because there is only one valid user</t>
+    <t>As a tester I cannot execute this test because there is only one valid user</t>
   </si>
   <si>
     <t>Sec_001</t>
   </si>
   <si>
     <t>Security Testing</t>
+  </si>
+  <si>
+    <t>TC_049</t>
   </si>
   <si>
     <t>Trying to access protected routes without authentication</t>
@@ -1388,7 +1504,10 @@
 2. User is redirected to login page or shown an appropriate error message</t>
   </si>
   <si>
-    <t>TThere are no protected routes. When user logs in they are not redirected to any page</t>
+    <t>There are no protected routes. When user logs in they are not redirected to any page</t>
+  </si>
+  <si>
+    <t>TC_050</t>
   </si>
   <si>
     <t>Test SQL injection on lookup fields</t>
@@ -1416,6 +1535,9 @@
     <t>The application is not connected to a database, so this threat does not affect it</t>
   </si>
   <si>
+    <t>TC_051</t>
+  </si>
+  <si>
     <t>Verify the use of HTTPS in all communications</t>
   </si>
   <si>
@@ -1438,6 +1560,9 @@
     <t xml:space="preserve">The application do not  use HTTPS, it is in localhost, but when it connects to the server it is on HTTP </t>
   </si>
   <si>
+    <t>TC_052</t>
+  </si>
+  <si>
     <t>Check secure password handling (hashing)</t>
   </si>
   <si>
@@ -1463,6 +1588,9 @@
     <t>User password is hardcoded in the source code. It it not allowed to register a new user, nor change the passwor</t>
   </si>
   <si>
+    <t>TC_053</t>
+  </si>
+  <si>
     <t>Try to manipulate product prices from the frontend</t>
   </si>
   <si>
@@ -1494,6 +1622,9 @@
     <t>Compatibility Testing</t>
   </si>
   <si>
+    <t>TC_054</t>
+  </si>
+  <si>
     <t>Check functionality in Chrome and Edge</t>
   </si>
   <si>
@@ -1515,6 +1646,9 @@
     <t xml:space="preserve">Funcionalities work as expected, but in Edge image is bigger, considering having the same Zoom porcentages </t>
   </si>
   <si>
+    <t>TC_055</t>
+  </si>
+  <si>
     <t>Test responsiveness on mobile devices (iOS and Android)</t>
   </si>
   <si>
@@ -1537,6 +1671,9 @@
     <t>I cannot render the application on cell phones but I tested it with DevTools an I could see the responsiveness</t>
   </si>
   <si>
+    <t>TC_056</t>
+  </si>
+  <si>
     <t>Check display on different screen sizes</t>
   </si>
   <si>
@@ -1568,6 +1705,9 @@
     <t>Data integrity testing</t>
   </si>
   <si>
+    <t>TC_057</t>
+  </si>
+  <si>
     <t>Verify that order totals are calculated correctly</t>
   </si>
   <si>
@@ -1595,6 +1735,9 @@
 2. Users cannot see shopping cart</t>
   </si>
   <si>
+    <t>TC_058</t>
+  </si>
+  <si>
     <t>Verify that inventory changes are appropriately reflected after orders</t>
   </si>
   <si>
@@ -1620,6 +1763,9 @@
 2. User cannot place  an order for a product</t>
   </si>
   <si>
+    <t>TC_059</t>
+  </si>
+  <si>
     <t>Ensure user information remains consistent between sessions</t>
   </si>
   <si>
@@ -1651,6 +1797,9 @@
     <t>Usability Testing</t>
   </si>
   <si>
+    <t>TC_060</t>
+  </si>
+  <si>
     <t>Evaluate the ease of navigation in the ReactJS dashboard</t>
   </si>
   <si>
@@ -1677,6 +1826,9 @@
 2. Navigation structure is lconfusing</t>
   </si>
   <si>
+    <t>TC_061</t>
+  </si>
+  <si>
     <t>Check the intuitiveness of the purchasing process in Aurelia</t>
   </si>
   <si>
@@ -1702,6 +1854,9 @@
     <t xml:space="preserve"> 1. Users cannot complete a purchase</t>
   </si>
   <si>
+    <t>TC_062</t>
+  </si>
+  <si>
     <t>Verify that error messages are clear and useful</t>
   </si>
   <si>
@@ -1733,6 +1888,9 @@
     <t>White Box Testing</t>
   </si>
   <si>
+    <t>TC_063</t>
+  </si>
+  <si>
     <t>Verify product filtering algorithm</t>
   </si>
   <si>
@@ -1754,6 +1912,9 @@
   </si>
   <si>
     <t>Both in the "ProductList.js" and in the "ProductController.cs" files, there is no algorithm that filters products by category</t>
+  </si>
+  <si>
+    <t>TC_064</t>
   </si>
   <si>
     <t>Validate shopping cart total calculation</t>
@@ -1781,6 +1942,9 @@
     <t>Both in the "OrderList.js" and in the "OrderController.cs" files, there is no algorithm that adds products to cart</t>
   </si>
   <si>
+    <t>TC_065</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Check order processing workflow</t>
   </si>
   <si>
@@ -1804,6 +1968,9 @@
     <t>The system does not have implemented all the methods needed in a complete CRUD an user cannot do any of the operations, the only functionality implemented in the frontend is user login</t>
   </si>
   <si>
+    <t>TC_066</t>
+  </si>
+  <si>
     <t>Evaluate authentication middleware</t>
   </si>
   <si>
@@ -1828,6 +1995,9 @@
     <t>The system lacks of authentication middleware. Valid username and password are hardcoded</t>
   </si>
   <si>
+    <t>TC_067</t>
+  </si>
+  <si>
     <t>Test database connection pool management</t>
   </si>
   <si>
@@ -1850,7 +2020,7 @@
 3. Unused connections are properly closed and returned to the pool</t>
   </si>
   <si>
-    <t>The sistem does not have implemented a database connection and it is stateless, does not keep any information and when the application restarts all the information disappears</t>
+    <t>The system does not have implemented a database connection and it is stateless, does not keep any information and when the application restarts all the information disappears</t>
   </si>
 </sst>
 </file>
@@ -2254,7 +2424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2459,6 +2629,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6217,8 +6390,8 @@
   </sheetPr>
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6825,8 +6998,8 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6917,34 +7090,34 @@
     </row>
     <row r="7" spans="1:11" ht="72.75">
       <c r="A7" s="19" t="s">
-        <v>405</v>
+        <v>452</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>406</v>
+        <v>453</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>407</v>
+        <v>454</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>455</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>408</v>
+        <v>456</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>409</v>
+        <v>457</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>410</v>
+        <v>458</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>411</v>
+        <v>459</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>412</v>
+        <v>460</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>413</v>
+        <v>461</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>50</v>
@@ -6952,34 +7125,34 @@
     </row>
     <row r="8" spans="1:11" ht="102" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>405</v>
+        <v>452</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>406</v>
+        <v>453</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>414</v>
+        <v>463</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>415</v>
+        <v>464</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>416</v>
+        <v>465</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>417</v>
+        <v>466</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>418</v>
+        <v>467</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>419</v>
+        <v>468</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>420</v>
+        <v>469</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -6987,34 +7160,34 @@
     </row>
     <row r="9" spans="1:11" ht="99" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>405</v>
+        <v>452</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>406</v>
+        <v>453</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>470</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>421</v>
+        <v>471</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>422</v>
+        <v>472</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>423</v>
+        <v>473</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>424</v>
+        <v>474</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>425</v>
+        <v>475</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>426</v>
+        <v>476</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>427</v>
+        <v>477</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -7038,8 +7211,8 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7130,34 +7303,34 @@
     </row>
     <row r="7" spans="1:11" ht="91.5" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>428</v>
+        <v>478</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>429</v>
+        <v>479</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>480</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>430</v>
+        <v>481</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>431</v>
+        <v>482</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>432</v>
+        <v>483</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>433</v>
+        <v>484</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>434</v>
+        <v>485</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>435</v>
+        <v>486</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>436</v>
+        <v>487</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>50</v>
@@ -7165,34 +7338,34 @@
     </row>
     <row r="8" spans="1:11" ht="104.25" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>428</v>
+        <v>478</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>429</v>
+        <v>479</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>488</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>437</v>
+        <v>489</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>438</v>
+        <v>490</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>439</v>
+        <v>491</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>440</v>
+        <v>492</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>441</v>
+        <v>493</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>442</v>
+        <v>494</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>443</v>
+        <v>495</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -7200,34 +7373,34 @@
     </row>
     <row r="9" spans="1:11" ht="95.25" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>428</v>
+        <v>478</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>429</v>
+        <v>479</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>496</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>444</v>
+        <v>497</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>445</v>
+        <v>498</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>446</v>
+        <v>499</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>447</v>
+        <v>500</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>448</v>
+        <v>501</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>449</v>
+        <v>502</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>450</v>
+        <v>503</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -7266,8 +7439,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="H2" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7358,34 +7531,34 @@
     </row>
     <row r="7" spans="1:11" ht="112.5" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>451</v>
+        <v>504</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>452</v>
+        <v>505</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>506</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>453</v>
+        <v>507</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>454</v>
+        <v>508</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>455</v>
+        <v>509</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>456</v>
+        <v>510</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>457</v>
+        <v>511</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>458</v>
+        <v>512</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>459</v>
+        <v>513</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>50</v>
@@ -7393,34 +7566,34 @@
     </row>
     <row r="8" spans="1:11" ht="120.75" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>451</v>
+        <v>504</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>452</v>
+        <v>505</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>514</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>460</v>
+        <v>515</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>461</v>
+        <v>516</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>462</v>
+        <v>517</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>463</v>
+        <v>518</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>464</v>
+        <v>519</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>465</v>
+        <v>520</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -7428,34 +7601,34 @@
     </row>
     <row r="9" spans="1:11" ht="106.5" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>451</v>
+        <v>504</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>452</v>
+        <v>505</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>522</v>
       </c>
       <c r="D9" s="72" t="s">
-        <v>467</v>
+        <v>523</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>468</v>
+        <v>524</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>469</v>
+        <v>525</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>470</v>
+        <v>526</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>471</v>
+        <v>527</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>472</v>
+        <v>528</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>473</v>
+        <v>529</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -7463,34 +7636,34 @@
     </row>
     <row r="10" spans="1:11" ht="89.25" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>451</v>
+        <v>504</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>452</v>
+        <v>505</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>530</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>474</v>
+        <v>531</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>475</v>
+        <v>532</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>476</v>
+        <v>533</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>477</v>
+        <v>534</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>478</v>
+        <v>535</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>479</v>
+        <v>536</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>480</v>
+        <v>537</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>50</v>
@@ -7498,34 +7671,34 @@
     </row>
     <row r="11" spans="1:11" ht="105" customHeight="1">
       <c r="A11" s="20" t="s">
-        <v>451</v>
+        <v>504</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>452</v>
+        <v>505</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>43</v>
+        <v>538</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>481</v>
+        <v>539</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>482</v>
+        <v>540</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>483</v>
+        <v>541</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>484</v>
+        <v>542</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>485</v>
+        <v>543</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>486</v>
+        <v>544</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>487</v>
+        <v>545</v>
       </c>
       <c r="K11" s="54" t="s">
         <v>50</v>
@@ -7549,8 +7722,8 @@
   </sheetPr>
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="G12" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7645,28 +7818,28 @@
         <v>74</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>50</v>
@@ -7680,28 +7853,28 @@
         <v>74</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -7715,28 +7888,28 @@
         <v>74</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -7750,28 +7923,28 @@
         <v>74</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="I10" s="14" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>50</v>
@@ -7785,28 +7958,28 @@
         <v>74</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="K11" s="54" t="s">
         <v>50</v>
@@ -7833,28 +8006,28 @@
         <v>74</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="K12" s="54" t="s">
         <v>50</v>
@@ -7868,28 +8041,28 @@
         <v>74</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="K13" s="54" t="s">
         <v>50</v>
@@ -7903,28 +8076,28 @@
         <v>74</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="K14" s="43" t="s">
         <v>50</v>
@@ -7948,8 +8121,8 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7963,7 +8136,7 @@
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
     <col min="9" max="9" width="35.28515625" customWidth="1"/>
     <col min="10" max="10" width="52.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
@@ -8039,34 +8212,34 @@
     </row>
     <row r="7" spans="1:11" ht="102.75" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="K7" s="55" t="s">
         <v>50</v>
@@ -8074,34 +8247,34 @@
     </row>
     <row r="8" spans="1:11" ht="105.75" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -8109,34 +8282,34 @@
     </row>
     <row r="9" spans="1:11" ht="109.5" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="I9" s="52" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -8144,34 +8317,34 @@
     </row>
     <row r="10" spans="1:11" ht="84.75" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>50</v>
@@ -8179,34 +8352,34 @@
     </row>
     <row r="11" spans="1:11" ht="99" customHeight="1">
       <c r="A11" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="K11" s="54" t="s">
         <v>50</v>
@@ -8214,34 +8387,34 @@
     </row>
     <row r="12" spans="1:11" ht="113.25" customHeight="1">
       <c r="A12" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>51</v>
+        <v>179</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="K12" s="54" t="s">
         <v>50</v>
@@ -8249,34 +8422,34 @@
     </row>
     <row r="13" spans="1:11" ht="97.5" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="K13" s="54" t="s">
         <v>50</v>
@@ -8300,8 +8473,8 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="H15" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8392,34 +8565,34 @@
     </row>
     <row r="7" spans="1:11" ht="68.25" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>197</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="K7" s="55" t="s">
         <v>50</v>
@@ -8427,34 +8600,34 @@
     </row>
     <row r="8" spans="1:11" ht="72" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>205</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="K8" s="57" t="s">
         <v>27</v>
@@ -8462,34 +8635,34 @@
     </row>
     <row r="9" spans="1:11" ht="83.25" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>211</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="K9" s="58" t="s">
         <v>27</v>
@@ -8497,34 +8670,34 @@
     </row>
     <row r="10" spans="1:11" ht="99" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>50</v>
@@ -8532,34 +8705,34 @@
     </row>
     <row r="11" spans="1:11" ht="43.5">
       <c r="A11" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>43</v>
+        <v>226</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="K11" s="54" t="s">
         <v>50</v>
@@ -8567,34 +8740,34 @@
     </row>
     <row r="12" spans="1:11" ht="87">
       <c r="A12" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>51</v>
+        <v>233</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>217</v>
+        <v>238</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="K12" s="54" t="s">
         <v>50</v>
@@ -8602,34 +8775,34 @@
     </row>
     <row r="13" spans="1:11" ht="71.25" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>56</v>
+        <v>240</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="K13" s="54" t="s">
         <v>50</v>
@@ -8637,34 +8810,34 @@
     </row>
     <row r="14" spans="1:11" ht="96.75" customHeight="1">
       <c r="A14" s="36" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>62</v>
+        <v>247</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="K14" s="43" t="s">
         <v>50</v>
@@ -8672,34 +8845,34 @@
     </row>
     <row r="15" spans="1:11" ht="141" customHeight="1">
       <c r="A15" s="39" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>68</v>
+        <v>255</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="K15" s="59" t="s">
         <v>50</v>
@@ -8723,8 +8896,8 @@
   </sheetPr>
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8816,34 +8989,34 @@
     </row>
     <row r="7" spans="1:13" ht="96" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>265</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>50</v>
@@ -8851,34 +9024,34 @@
     </row>
     <row r="8" spans="1:13" ht="85.5" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>272</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -8886,34 +9059,34 @@
     </row>
     <row r="9" spans="1:13" ht="102" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="D9" s="72" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -8921,34 +9094,34 @@
     </row>
     <row r="10" spans="1:13" ht="120.75" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>50</v>
@@ -8956,34 +9129,34 @@
     </row>
     <row r="11" spans="1:13" ht="111" customHeight="1">
       <c r="A11" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>43</v>
+        <v>296</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>268</v>
+        <v>297</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>270</v>
+        <v>299</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>272</v>
+        <v>301</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>273</v>
+        <v>302</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>274</v>
+        <v>303</v>
       </c>
       <c r="K11" s="54" t="s">
         <v>50</v>
@@ -8991,34 +9164,34 @@
     </row>
     <row r="12" spans="1:13" ht="119.25" customHeight="1">
       <c r="A12" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>51</v>
+        <v>304</v>
       </c>
       <c r="D12" s="71" t="s">
-        <v>275</v>
+        <v>305</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>279</v>
+        <v>309</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="K12" s="54" t="s">
         <v>50</v>
@@ -9026,34 +9199,34 @@
     </row>
     <row r="13" spans="1:13" ht="114" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>56</v>
+        <v>311</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>285</v>
+        <v>316</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="K13" s="54" t="s">
         <v>50</v>
@@ -9061,34 +9234,34 @@
     </row>
     <row r="14" spans="1:13" ht="113.25" customHeight="1">
       <c r="A14" s="20" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>62</v>
+        <v>319</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>288</v>
+        <v>320</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>291</v>
+        <v>323</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>292</v>
+        <v>324</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>293</v>
+        <v>325</v>
       </c>
       <c r="J14" s="60" t="s">
-        <v>294</v>
+        <v>326</v>
       </c>
       <c r="K14" s="54" t="s">
         <v>50</v>
@@ -9096,34 +9269,34 @@
     </row>
     <row r="15" spans="1:13" ht="105" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>68</v>
+        <v>327</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>295</v>
+        <v>328</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>296</v>
+        <v>329</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>298</v>
+        <v>331</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>299</v>
+        <v>332</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="J15" s="60" t="s">
-        <v>301</v>
+        <v>333</v>
+      </c>
+      <c r="J15" s="76" t="s">
+        <v>334</v>
       </c>
       <c r="K15" s="61" t="s">
         <v>50</v>
@@ -9147,8 +9320,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="I6" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9213,7 +9386,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>302</v>
+        <v>335</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>10</v>
@@ -9239,34 +9412,34 @@
     </row>
     <row r="7" spans="1:11" ht="94.5" customHeight="1">
       <c r="A7" s="35" t="s">
-        <v>303</v>
+        <v>336</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>19</v>
+        <v>338</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>305</v>
+        <v>339</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>306</v>
+        <v>340</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>308</v>
+        <v>342</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="K7" s="43" t="s">
         <v>50</v>
@@ -9274,34 +9447,34 @@
     </row>
     <row r="8" spans="1:11" ht="116.25" customHeight="1">
       <c r="A8" s="36" t="s">
-        <v>303</v>
+        <v>336</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>28</v>
+        <v>346</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>312</v>
+        <v>347</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>313</v>
+        <v>348</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>314</v>
+        <v>349</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>315</v>
+        <v>350</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>317</v>
+        <v>352</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>318</v>
+        <v>353</v>
       </c>
       <c r="K8" s="43" t="s">
         <v>50</v>
@@ -9309,34 +9482,34 @@
     </row>
     <row r="9" spans="1:11" ht="116.25" customHeight="1">
       <c r="A9" s="36" t="s">
-        <v>303</v>
+        <v>336</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>35</v>
+        <v>354</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>319</v>
+        <v>355</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>321</v>
+        <v>357</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>322</v>
+        <v>358</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>323</v>
+        <v>359</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>325</v>
+        <v>361</v>
       </c>
       <c r="K9" s="43" t="s">
         <v>50</v>
@@ -9363,8 +9536,8 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9455,34 +9628,34 @@
     </row>
     <row r="7" spans="1:11" ht="117.75" customHeight="1">
       <c r="A7" s="35" t="s">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>327</v>
+        <v>363</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>19</v>
+        <v>364</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>329</v>
+        <v>366</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>330</v>
+        <v>367</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>331</v>
+        <v>368</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>332</v>
+        <v>369</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>333</v>
+        <v>370</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="K7" s="43" t="s">
         <v>50</v>
@@ -9490,34 +9663,34 @@
     </row>
     <row r="8" spans="1:11" ht="87">
       <c r="A8" s="36" t="s">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>327</v>
+        <v>363</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>28</v>
+        <v>372</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>335</v>
+        <v>373</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>336</v>
+        <v>374</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>337</v>
+        <v>375</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>338</v>
+        <v>376</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>339</v>
+        <v>377</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>340</v>
+        <v>378</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="K8" s="43" t="s">
         <v>50</v>
@@ -9525,34 +9698,34 @@
     </row>
     <row r="9" spans="1:11" ht="124.5" customHeight="1">
       <c r="A9" s="36" t="s">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>327</v>
+        <v>363</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>35</v>
+        <v>379</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>341</v>
+        <v>380</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>343</v>
+        <v>382</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>345</v>
+        <v>384</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>347</v>
+        <v>386</v>
       </c>
       <c r="K9" s="43" t="s">
         <v>50</v>
@@ -9576,8 +9749,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9668,34 +9841,34 @@
     </row>
     <row r="7" spans="1:11" ht="112.5" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>389</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>350</v>
+        <v>390</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>351</v>
+        <v>391</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>352</v>
+        <v>392</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>353</v>
+        <v>393</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>354</v>
+        <v>394</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>355</v>
+        <v>395</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>356</v>
+        <v>396</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>50</v>
@@ -9703,34 +9876,34 @@
     </row>
     <row r="8" spans="1:11" ht="120.75" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>397</v>
       </c>
       <c r="D8" s="71" t="s">
-        <v>357</v>
+        <v>398</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>358</v>
+        <v>399</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>359</v>
+        <v>400</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>360</v>
+        <v>401</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>361</v>
+        <v>402</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>362</v>
+        <v>403</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>363</v>
+        <v>404</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>50</v>
@@ -9738,34 +9911,34 @@
     </row>
     <row r="9" spans="1:11" ht="106.5" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>405</v>
       </c>
       <c r="D9" s="70" t="s">
-        <v>364</v>
+        <v>406</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>365</v>
+        <v>407</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>366</v>
+        <v>408</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>367</v>
+        <v>409</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>368</v>
+        <v>410</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>369</v>
+        <v>411</v>
       </c>
       <c r="K9" s="54" t="s">
         <v>50</v>
@@ -9773,34 +9946,34 @@
     </row>
     <row r="10" spans="1:11" ht="89.25" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>412</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>50</v>
@@ -9808,34 +9981,34 @@
     </row>
     <row r="11" spans="1:11" ht="93.75" customHeight="1">
       <c r="A11" s="20" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>43</v>
+        <v>420</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>377</v>
+        <v>421</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>378</v>
+        <v>422</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>379</v>
+        <v>423</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>380</v>
+        <v>424</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>381</v>
+        <v>425</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>382</v>
+        <v>426</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>383</v>
+        <v>427</v>
       </c>
       <c r="K11" s="54" t="s">
         <v>50</v>
@@ -9859,8 +10032,8 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="G8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9951,34 +10124,34 @@
     </row>
     <row r="7" spans="1:11" ht="87.75" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>384</v>
+        <v>428</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>385</v>
+        <v>429</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>430</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>386</v>
+        <v>431</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>387</v>
+        <v>432</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>388</v>
+        <v>433</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>389</v>
+        <v>434</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>390</v>
+        <v>435</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>391</v>
+        <v>436</v>
       </c>
       <c r="K7" s="58" t="s">
         <v>27</v>
@@ -9986,34 +10159,34 @@
     </row>
     <row r="8" spans="1:11" ht="98.25" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>384</v>
+        <v>428</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>385</v>
+        <v>429</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>28</v>
+        <v>437</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>392</v>
+        <v>438</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>393</v>
+        <v>439</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>394</v>
+        <v>440</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>395</v>
+        <v>441</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>396</v>
+        <v>442</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>397</v>
+        <v>443</v>
       </c>
       <c r="K8" s="58" t="s">
         <v>27</v>
@@ -10021,34 +10194,34 @@
     </row>
     <row r="9" spans="1:11" ht="105.75" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>384</v>
+        <v>428</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>385</v>
+        <v>429</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>444</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>398</v>
+        <v>445</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>399</v>
+        <v>446</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>400</v>
+        <v>447</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>401</v>
+        <v>448</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>402</v>
+        <v>449</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>403</v>
+        <v>450</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>404</v>
+        <v>451</v>
       </c>
       <c r="K9" s="58" t="s">
         <v>27</v>

</xml_diff>